<commit_message>
Operations charts, performance eval 2 implemented
</commit_message>
<xml_diff>
--- a/charts/chartdata.xlsx
+++ b/charts/chartdata.xlsx
@@ -8,44 +8,44 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b53d5d4b50337fb/Documents/CUNY/matrix-multiplication/charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{789D5A4D-32CF-944F-8736-A7A558B9D8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{789D5A4D-32CF-944F-8736-A7A558B9D8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F262B0E3-8B58-E945-9056-66CA27BB388E}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="500" windowWidth="21400" windowHeight="17500" xr2:uid="{50D41231-1AC9-314E-B928-DD39809BD5E5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Operations" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$16</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$17:$A$27</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$16</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$17:$C$27</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$A$16</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$A$17:$A$27</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$17:$B$27</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$C$16</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$C$17:$C$27</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$A$16</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$A$17:$A$27</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$B$17:$B$27</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$16</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$C$17:$C$27</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$A$16</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$A$17:$A$27</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$B$17:$B$27</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$C$16</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$C$17:$C$27</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$17:$B$27</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$16</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$17:$C$27</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$16</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$17:$A$27</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$17:$B$27</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Operations!$A$16</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Operations!$A$17:$A$27</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Operations!$C$16</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Operations!$C$17:$C$27</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Operations!$A$16</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Operations!$A$17:$A$27</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Operations!$B$16</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Operations!$B$17:$B$27</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Operations!$C$16</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Operations!$C$17:$C$27</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Operations!$A$16</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Operations!$A$17:$A$27</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Operations!$B$16</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Operations!$B$16</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Operations!$B$17:$B$27</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Operations!$C$16</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Operations!$C$17:$C$27</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Operations!$A$16</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Operations!$A$17:$A$27</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Operations!$B$16</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Operations!$B$17:$B$27</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Operations!$C$16</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Operations!$C$17:$C$27</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Operations!$B$17:$B$27</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Operations!$C$16</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Operations!$C$17:$C$27</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Operations!$A$16</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Operations!$A$17:$A$27</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Operations!$B$16</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Operations!$B$17:$B$27</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -261,7 +261,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$16</c:f>
+              <c:f>Operations!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -284,7 +284,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$27</c:f>
+              <c:f>Operations!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -326,7 +326,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$27</c:f>
+              <c:f>Operations!$B$17:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -378,7 +378,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$16</c:f>
+              <c:f>Operations!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -401,7 +401,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$27</c:f>
+              <c:f>Operations!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -443,7 +443,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$27</c:f>
+              <c:f>Operations!$C$17:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -876,7 +876,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$16</c:f>
+              <c:f>Operations!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -899,7 +899,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$31:$A$41</c:f>
+              <c:f>Operations!$A$31:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -941,7 +941,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$31:$B$41</c:f>
+              <c:f>Operations!$B$31:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -993,7 +993,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$16</c:f>
+              <c:f>Operations!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1016,7 +1016,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$31:$A$41</c:f>
+              <c:f>Operations!$A$31:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1058,7 +1058,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$31:$C$41</c:f>
+              <c:f>Operations!$C$31:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1491,7 +1491,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$16</c:f>
+              <c:f>Operations!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1514,7 +1514,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$45:$A$55</c:f>
+              <c:f>Operations!$A$45:$A$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1556,7 +1556,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$45:$B$55</c:f>
+              <c:f>Operations!$B$45:$B$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1608,7 +1608,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$16</c:f>
+              <c:f>Operations!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1631,7 +1631,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$45:$A$55</c:f>
+              <c:f>Operations!$A$45:$A$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1673,7 +1673,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$45:$C$55</c:f>
+              <c:f>Operations!$C$45:$C$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4111,7 +4111,7 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>